<commit_message>
save the prediction of each trade inside csv file
</commit_message>
<xml_diff>
--- a/saved_model/results/15_min.xlsx
+++ b/saved_model/results/15_min.xlsx
@@ -382,16 +382,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-412.0839910812398</v>
+        <v>-746.7475945882428</v>
       </c>
       <c r="C2">
-        <v>13.70442432958295</v>
+        <v>15.68323435625896</v>
       </c>
       <c r="D2">
-        <v>1.398223538119911</v>
+        <v>1.30481513327601</v>
       </c>
       <c r="E2">
-        <v>23642</v>
+        <v>34183</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -399,16 +399,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-74.0363588495952</v>
+        <v>-570.3977028459137</v>
       </c>
       <c r="C3">
-        <v>2.351846368596929</v>
+        <v>11.76935229067931</v>
       </c>
       <c r="D3">
-        <v>1.297520661157025</v>
+        <v>1.322748267898383</v>
       </c>
       <c r="E3">
-        <v>23641</v>
+        <v>34182</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -416,16 +416,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-281.7746134929893</v>
+        <v>-427.7585592015432</v>
       </c>
       <c r="C4">
-        <v>10.84602368866328</v>
+        <v>10.55849741084228</v>
       </c>
       <c r="D4">
-        <v>1.307830783078308</v>
+        <v>1.323889246619446</v>
       </c>
       <c r="E4">
-        <v>23640</v>
+        <v>34181</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>

<commit_message>
remvoing bug where we always output the same prediction
</commit_message>
<xml_diff>
--- a/saved_model/results/15_min.xlsx
+++ b/saved_model/results/15_min.xlsx
@@ -357,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -382,16 +382,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-746.7475945882428</v>
+        <v>-583.8945067295343</v>
       </c>
       <c r="C2">
-        <v>15.68323435625896</v>
+        <v>21.90919926319211</v>
       </c>
       <c r="D2">
-        <v>1.30481513327601</v>
+        <v>1.083462132921175</v>
       </c>
       <c r="E2">
-        <v>34183</v>
+        <v>18458</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -399,16 +399,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-570.3977028459137</v>
+        <v>-375.2425857536614</v>
       </c>
       <c r="C3">
-        <v>11.76935229067931</v>
+        <v>17.02335157392859</v>
       </c>
       <c r="D3">
-        <v>1.322748267898383</v>
+        <v>1.17439446366782</v>
       </c>
       <c r="E3">
-        <v>34182</v>
+        <v>18457</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -416,16 +416,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-427.7585592015432</v>
+        <v>-309.4941282964456</v>
       </c>
       <c r="C4">
-        <v>10.55849741084228</v>
+        <v>12.93346337234504</v>
       </c>
       <c r="D4">
-        <v>1.323889246619446</v>
+        <v>1.226679104477612</v>
       </c>
       <c r="E4">
-        <v>34181</v>
+        <v>18456</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -433,16 +433,220 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-70.82719239390551</v>
+        <v>-235.2131625981372</v>
       </c>
       <c r="C5">
-        <v>6.624645712593595</v>
+        <v>9.536710918450284</v>
       </c>
       <c r="D5">
-        <v>1.409230769230769</v>
+        <v>1.205513784461153</v>
       </c>
       <c r="E5">
-        <v>23639</v>
+        <v>18455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-287.6495036159624</v>
+      </c>
+      <c r="C6">
+        <v>9.846103825728839</v>
+      </c>
+      <c r="D6">
+        <v>1.057757644394111</v>
+      </c>
+      <c r="E6">
+        <v>18454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-247.434345068912</v>
+      </c>
+      <c r="C7">
+        <v>8.822413699669431</v>
+      </c>
+      <c r="D7">
+        <v>1.167776298268975</v>
+      </c>
+      <c r="E7">
+        <v>18453</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-157.8501286614251</v>
+      </c>
+      <c r="C8">
+        <v>8.351398222414915</v>
+      </c>
+      <c r="D8">
+        <v>1.269513991163476</v>
+      </c>
+      <c r="E8">
+        <v>18452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-219.0863649459424</v>
+      </c>
+      <c r="C9">
+        <v>8.124220909435802</v>
+      </c>
+      <c r="D9">
+        <v>0.9646133682830931</v>
+      </c>
+      <c r="E9">
+        <v>18451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-116.822503001472</v>
+      </c>
+      <c r="C10">
+        <v>6.699186991869918</v>
+      </c>
+      <c r="D10">
+        <v>1.243194192377495</v>
+      </c>
+      <c r="E10">
+        <v>18450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-179.1598834748678</v>
+      </c>
+      <c r="C11">
+        <v>6.601983847363001</v>
+      </c>
+      <c r="D11">
+        <v>1.096385542168675</v>
+      </c>
+      <c r="E11">
+        <v>18449</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-292.8185644338039</v>
+      </c>
+      <c r="C12">
+        <v>6.526452732003469</v>
+      </c>
+      <c r="D12">
+        <v>0.8871473354231975</v>
+      </c>
+      <c r="E12">
+        <v>18448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-166.9050034017448</v>
+      </c>
+      <c r="C13">
+        <v>5.849189570119803</v>
+      </c>
+      <c r="D13">
+        <v>1.111545988258317</v>
+      </c>
+      <c r="E13">
+        <v>18447</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-218.4570402655779</v>
+      </c>
+      <c r="C14">
+        <v>5.665184863927139</v>
+      </c>
+      <c r="D14">
+        <v>0.9387755102040817</v>
+      </c>
+      <c r="E14">
+        <v>18446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>-228.4948665390954</v>
+      </c>
+      <c r="C18">
+        <v>4.777139138922026</v>
+      </c>
+      <c r="D18">
+        <v>0.8430962343096234</v>
+      </c>
+      <c r="E18">
+        <v>18442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>-241.9085060696412</v>
+      </c>
+      <c r="C19">
+        <v>4.576758310286861</v>
+      </c>
+      <c r="D19">
+        <v>0.7805907172995781</v>
+      </c>
+      <c r="E19">
+        <v>18441</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>60.8864454667772</v>
+      </c>
+      <c r="C20">
+        <v>4.202819956616052</v>
+      </c>
+      <c r="D20">
+        <v>1.327327327327327</v>
+      </c>
+      <c r="E20">
+        <v>18440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>